<commit_message>
P08/: Updated scrum sheet
</commit_message>
<xml_diff>
--- a/P08/JADE_Scrum_Sprint_2.xlsx
+++ b/P08/JADE_Scrum_Sprint_2.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\WASEE\Google Drive\Code\UVM\cse1325\P07\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/waseem/Documents/SchoolCode/cse1325/P08/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5D7CF1C-1C93-4262-84D8-570BD34F7B09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D061E405-5268-764F-9FC7-9449EEDF7736}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
-    <sheet name="Sprint 01 Backlog" sheetId="2" r:id="rId2"/>
-    <sheet name="Sprint 02 Backlog" sheetId="3" r:id="rId3"/>
-    <sheet name="Sprint 03 Backlog" sheetId="4" r:id="rId4"/>
+    <sheet name="Sprint 03 Backlog" sheetId="4" r:id="rId2"/>
+    <sheet name="Sprint 01 Backlog" sheetId="2" r:id="rId3"/>
+    <sheet name="Sprint 02 Backlog" sheetId="3" r:id="rId4"/>
     <sheet name="Sprint 04 Backlog" sheetId="5" r:id="rId5"/>
     <sheet name="Sprint 05 Backlog" sheetId="6" r:id="rId6"/>
     <sheet name="Sprint 06 Backlog" sheetId="7" r:id="rId7"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="507" uniqueCount="227">
   <si>
     <t>Product Name:</t>
   </si>
@@ -658,6 +658,69 @@
   </si>
   <si>
     <t>Create an about dialog with the logo, prgram version and copyright, along with  appropriate creditation</t>
+  </si>
+  <si>
+    <t>Create a "New" menuItem under file</t>
+  </si>
+  <si>
+    <t>Create a "New" button in the toolbar</t>
+  </si>
+  <si>
+    <t>Completed Day 1</t>
+  </si>
+  <si>
+    <t>Create a onNewClick method that will be called when new button and menu option are clicked</t>
+  </si>
+  <si>
+    <t>Create a save menuitem under file menu</t>
+  </si>
+  <si>
+    <t>Create a save button in the toolbar</t>
+  </si>
+  <si>
+    <t>create a onSaveClick to be called when save is clicked</t>
+  </si>
+  <si>
+    <t>Create an Open menu item under file</t>
+  </si>
+  <si>
+    <t>create an Open button in the toolbar</t>
+  </si>
+  <si>
+    <t>create a onOpenClick method to be called when Open is clicked</t>
+  </si>
+  <si>
+    <t>Create a Save As opetion under the file menu</t>
+  </si>
+  <si>
+    <t>Create a Save As button in the toolbar</t>
+  </si>
+  <si>
+    <t>Create a onSaveAsClick method to be called when save as is clicked</t>
+  </si>
+  <si>
+    <t>Create a save mothod for the store class</t>
+  </si>
+  <si>
+    <t>Create an open method for the store class</t>
+  </si>
+  <si>
+    <t>Create a save method for the Product class</t>
+  </si>
+  <si>
+    <t>Create a save method for the Donut class</t>
+  </si>
+  <si>
+    <t>Create an open method for the Donut class</t>
+  </si>
+  <si>
+    <t>Create a save method for the Java class</t>
+  </si>
+  <si>
+    <t>Create an open method for the Java class</t>
+  </si>
+  <si>
+    <t>Create an open mehotd for the Product class</t>
   </si>
 </sst>
 </file>
@@ -1444,6 +1507,319 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
+              <c:f>'Sprint 03 Backlog'!$B$7:$B$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>16</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-E67F-4962-B05B-09A2542B5EC4}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:hiLowLines>
+          <c:spPr>
+            <a:ln w="0">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:hiLowLines>
+        <c:smooth val="0"/>
+        <c:axId val="13648043"/>
+        <c:axId val="31276611"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="13648043"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" strike="noStrike" spc="-1">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="900" b="0" strike="noStrike" spc="-1">
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Days</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln w="0">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="0">
+            <a:solidFill>
+              <a:srgbClr val="B3B3B3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="31276611"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="31276611"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="0">
+              <a:solidFill>
+                <a:srgbClr val="B3B3B3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" strike="noStrike" spc="-1">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="900" b="0" strike="noStrike" spc="-1">
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Tasks</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln w="0">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="0">
+            <a:solidFill>
+              <a:srgbClr val="B3B3B3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="13648043"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:solidFill>
+            <a:srgbClr val="B3B3B3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="1"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="FFFFFF"/>
+    </a:solidFill>
+    <a:ln w="0">
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <c:style val="2"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1300" b="0" strike="noStrike" spc="-1">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1300" b="0" strike="noStrike" spc="-1">
+                <a:latin typeface="Arial"/>
+              </a:rPr>
+              <a:t>Sprint Burn Chart</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr wrap="none"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="1"/>
+            <c:separator> </c:separator>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
               <c:f>'Sprint 01 Backlog'!$B$7:$B$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
@@ -1666,7 +2042,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -1947,319 +2323,6 @@
           </a:p>
         </c:txPr>
         <c:crossAx val="96313299"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln w="0">
-          <a:solidFill>
-            <a:srgbClr val="B3B3B3"/>
-          </a:solidFill>
-        </a:ln>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="1"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:srgbClr val="FFFFFF"/>
-    </a:solidFill>
-    <a:ln w="0">
-      <a:noFill/>
-    </a:ln>
-  </c:spPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <c:style val="2"/>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1300" b="0" strike="noStrike" spc="-1">
-                <a:latin typeface="Arial"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US" sz="1300" b="0" strike="noStrike" spc="-1">
-                <a:latin typeface="Arial"/>
-              </a:rPr>
-              <a:t>Sprint Burn Chart</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln w="0">
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:spPr>
-            <a:ln w="28800">
-              <a:solidFill>
-                <a:srgbClr val="004586"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:dLbls>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr wrap="none"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
-                    <a:latin typeface="Arial"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="en-US"/>
-              </a:p>
-            </c:txPr>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="1"/>
-            <c:separator> </c:separator>
-            <c:showLeaderLines val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="1"/>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
-          <c:val>
-            <c:numRef>
-              <c:f>'Sprint 03 Backlog'!$B$7:$B$14</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-E67F-4962-B05B-09A2542B5EC4}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:hiLowLines>
-          <c:spPr>
-            <a:ln w="0">
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-        </c:hiLowLines>
-        <c:smooth val="0"/>
-        <c:axId val="13648043"/>
-        <c:axId val="31276611"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="13648043"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="900" b="0" strike="noStrike" spc="-1">
-                    <a:latin typeface="Arial"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US" sz="900" b="0" strike="noStrike" spc="-1">
-                    <a:latin typeface="Arial"/>
-                  </a:rPr>
-                  <a:t>Days</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln w="0">
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln w="0">
-            <a:solidFill>
-              <a:srgbClr val="B3B3B3"/>
-            </a:solidFill>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
-                <a:latin typeface="Arial"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="31276611"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="31276611"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="0">
-              <a:solidFill>
-                <a:srgbClr val="B3B3B3"/>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="900" b="0" strike="noStrike" spc="-1">
-                    <a:latin typeface="Arial"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US" sz="900" b="0" strike="noStrike" spc="-1">
-                    <a:latin typeface="Arial"/>
-                  </a:rPr>
-                  <a:t>Tasks</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln w="0">
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln w="0">
-            <a:solidFill>
-              <a:srgbClr val="B3B3B3"/>
-            </a:solidFill>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
-                <a:latin typeface="Arial"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="13648043"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3289,10 +3352,10 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1">
+        <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3333,7 +3396,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3371,10 +3434,10 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2">
+        <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3820,23 +3883,23 @@
   </sheetPr>
   <dimension ref="A1:AMJ79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K29" sqref="K28:K29"/>
+    <sheetView topLeftCell="A27" zoomScale="174" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="13.6640625" style="1" customWidth="1"/>
     <col min="2" max="2" width="11" style="1" customWidth="1"/>
-    <col min="3" max="3" width="8.5703125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="4.42578125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="8.42578125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="17.7109375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="8.85546875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="45.5703125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="39.140625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="53.7109375" style="1" customWidth="1"/>
-    <col min="11" max="1024" width="11.5703125" style="1"/>
+    <col min="3" max="3" width="8.5" style="1" customWidth="1"/>
+    <col min="4" max="4" width="4.5" style="1" customWidth="1"/>
+    <col min="5" max="5" width="8.5" style="1" customWidth="1"/>
+    <col min="6" max="6" width="17.6640625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="8.83203125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="45.5" style="1" customWidth="1"/>
+    <col min="9" max="9" width="39.1640625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="53.6640625" style="1" customWidth="1"/>
+    <col min="11" max="1024" width="11.5" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="4" customFormat="1" ht="18">
@@ -3856,7 +3919,7 @@
       </c>
       <c r="I1" s="37"/>
     </row>
-    <row r="2" spans="1:9" s="4" customFormat="1" ht="15.75">
+    <row r="2" spans="1:9" s="4" customFormat="1" ht="16">
       <c r="A2" s="24" t="s">
         <v>3</v>
       </c>
@@ -4221,7 +4284,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="24" spans="1:10">
+    <row r="24" spans="1:10" ht="14">
       <c r="A24" s="14" t="s">
         <v>30</v>
       </c>
@@ -4251,7 +4314,7 @@
       </c>
       <c r="J24" s="26"/>
     </row>
-    <row r="25" spans="1:10">
+    <row r="25" spans="1:10" ht="14">
       <c r="A25" s="14" t="s">
         <v>34</v>
       </c>
@@ -4281,7 +4344,7 @@
       </c>
       <c r="J25" s="26"/>
     </row>
-    <row r="26" spans="1:10">
+    <row r="26" spans="1:10" ht="14">
       <c r="A26" s="14" t="s">
         <v>37</v>
       </c>
@@ -4311,7 +4374,7 @@
       </c>
       <c r="J26" s="26"/>
     </row>
-    <row r="27" spans="1:10" ht="38.25">
+    <row r="27" spans="1:10" ht="28">
       <c r="A27" s="17" t="s">
         <v>40</v>
       </c>
@@ -4343,7 +4406,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="28" spans="1:10" ht="25.5">
+    <row r="28" spans="1:10" ht="28">
       <c r="A28" s="17" t="s">
         <v>44</v>
       </c>
@@ -4375,7 +4438,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="29" spans="1:10" s="21" customFormat="1" ht="25.5">
+    <row r="29" spans="1:10" s="21" customFormat="1" ht="28">
       <c r="A29" s="14" t="s">
         <v>47</v>
       </c>
@@ -4405,7 +4468,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="30" spans="1:10" s="21" customFormat="1" ht="25.5">
+    <row r="30" spans="1:10" s="21" customFormat="1" ht="28">
       <c r="A30" s="14" t="s">
         <v>51</v>
       </c>
@@ -4435,7 +4498,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="31" spans="1:10" s="21" customFormat="1" ht="25.5">
+    <row r="31" spans="1:10" s="21" customFormat="1" ht="28">
       <c r="A31" s="14" t="s">
         <v>54</v>
       </c>
@@ -4465,7 +4528,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="32" spans="1:10">
+    <row r="32" spans="1:10" ht="14">
       <c r="A32" s="24" t="s">
         <v>56</v>
       </c>
@@ -4495,7 +4558,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="33" spans="1:1024">
+    <row r="33" spans="1:1024" ht="14">
       <c r="A33" s="24" t="s">
         <v>61</v>
       </c>
@@ -5539,7 +5602,7 @@
       <c r="AMI33" s="24"/>
       <c r="AMJ33" s="24"/>
     </row>
-    <row r="34" spans="1:1024" ht="25.5">
+    <row r="34" spans="1:1024" ht="28">
       <c r="A34" s="17" t="s">
         <v>63</v>
       </c>
@@ -6583,7 +6646,7 @@
       <c r="AMI34" s="24"/>
       <c r="AMJ34" s="24"/>
     </row>
-    <row r="35" spans="1:1024" s="21" customFormat="1">
+    <row r="35" spans="1:1024" s="21" customFormat="1" ht="14">
       <c r="A35" s="17" t="s">
         <v>68</v>
       </c>
@@ -6611,7 +6674,7 @@
       </c>
       <c r="J35" s="20"/>
     </row>
-    <row r="36" spans="1:1024" s="21" customFormat="1">
+    <row r="36" spans="1:1024" s="21" customFormat="1" ht="14">
       <c r="A36" s="17" t="s">
         <v>72</v>
       </c>
@@ -6639,7 +6702,7 @@
       </c>
       <c r="J36" s="20"/>
     </row>
-    <row r="37" spans="1:1024" s="21" customFormat="1" ht="38.25">
+    <row r="37" spans="1:1024" s="21" customFormat="1" ht="28">
       <c r="A37" s="17" t="s">
         <v>75</v>
       </c>
@@ -6669,7 +6732,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="38" spans="1:1024" s="21" customFormat="1" ht="25.5">
+    <row r="38" spans="1:1024" s="21" customFormat="1" ht="28">
       <c r="A38" s="17" t="s">
         <v>79</v>
       </c>
@@ -6699,7 +6762,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="39" spans="1:1024" s="21" customFormat="1" ht="25.5">
+    <row r="39" spans="1:1024" s="21" customFormat="1" ht="14">
       <c r="A39" s="14" t="s">
         <v>83</v>
       </c>
@@ -6727,7 +6790,7 @@
       </c>
       <c r="J39" s="26"/>
     </row>
-    <row r="40" spans="1:1024" s="21" customFormat="1">
+    <row r="40" spans="1:1024" s="21" customFormat="1" ht="14">
       <c r="A40" s="14" t="s">
         <v>86</v>
       </c>
@@ -6755,7 +6818,7 @@
       </c>
       <c r="J40" s="26"/>
     </row>
-    <row r="41" spans="1:1024" s="22" customFormat="1" ht="25.5">
+    <row r="41" spans="1:1024" s="22" customFormat="1" ht="28">
       <c r="A41" s="14" t="s">
         <v>89</v>
       </c>
@@ -6785,7 +6848,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="42" spans="1:1024" ht="25.5">
+    <row r="42" spans="1:1024" ht="28">
       <c r="A42" s="24" t="s">
         <v>93</v>
       </c>
@@ -8873,7 +8936,7 @@
       <c r="AMI43" s="37"/>
       <c r="AMJ43" s="37"/>
     </row>
-    <row r="44" spans="1:1024" ht="25.5">
+    <row r="44" spans="1:1024" ht="14">
       <c r="A44" s="17" t="s">
         <v>100</v>
       </c>
@@ -10969,7 +11032,7 @@
       <c r="AMI47" s="14"/>
       <c r="AMJ47" s="14"/>
     </row>
-    <row r="48" spans="1:1024" ht="25.5">
+    <row r="48" spans="1:1024" ht="28">
       <c r="A48" s="24" t="s">
         <v>106</v>
       </c>
@@ -12009,7 +12072,7 @@
       <c r="AMI48" s="24"/>
       <c r="AMJ48" s="24"/>
     </row>
-    <row r="49" spans="1:10">
+    <row r="49" spans="1:10" ht="14">
       <c r="A49" s="24" t="s">
         <v>110</v>
       </c>
@@ -12033,7 +12096,7 @@
       </c>
       <c r="J49" s="26"/>
     </row>
-    <row r="50" spans="1:10" ht="38.25">
+    <row r="50" spans="1:10" ht="28">
       <c r="A50" s="24" t="s">
         <v>113</v>
       </c>
@@ -12057,7 +12120,7 @@
       </c>
       <c r="J50" s="26"/>
     </row>
-    <row r="51" spans="1:10">
+    <row r="51" spans="1:10" ht="14">
       <c r="A51" s="24" t="s">
         <v>116</v>
       </c>
@@ -12081,7 +12144,7 @@
       </c>
       <c r="J51" s="26"/>
     </row>
-    <row r="52" spans="1:10" ht="25.5">
+    <row r="52" spans="1:10" ht="28">
       <c r="A52" s="24" t="s">
         <v>119</v>
       </c>
@@ -12105,7 +12168,7 @@
       </c>
       <c r="J52" s="26"/>
     </row>
-    <row r="53" spans="1:10">
+    <row r="53" spans="1:10" ht="14">
       <c r="A53" s="24" t="s">
         <v>122</v>
       </c>
@@ -12155,7 +12218,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="55" spans="1:10" s="21" customFormat="1" ht="25.5">
+    <row r="55" spans="1:10" s="21" customFormat="1" ht="28">
       <c r="A55" s="14" t="s">
         <v>129</v>
       </c>
@@ -12181,7 +12244,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="56" spans="1:10" ht="25.5">
+    <row r="56" spans="1:10" ht="28">
       <c r="A56" s="24" t="s">
         <v>133</v>
       </c>
@@ -12205,7 +12268,7 @@
       </c>
       <c r="J56" s="26"/>
     </row>
-    <row r="57" spans="1:10" ht="25.5">
+    <row r="57" spans="1:10" ht="28">
       <c r="A57" s="24" t="s">
         <v>136</v>
       </c>
@@ -12229,7 +12292,7 @@
       </c>
       <c r="J57" s="26"/>
     </row>
-    <row r="58" spans="1:10" ht="25.5">
+    <row r="58" spans="1:10" ht="28">
       <c r="A58" s="24" t="s">
         <v>139</v>
       </c>
@@ -12253,7 +12316,7 @@
       </c>
       <c r="J58" s="26"/>
     </row>
-    <row r="59" spans="1:10" ht="38.25">
+    <row r="59" spans="1:10" ht="28">
       <c r="A59" s="24" t="s">
         <v>142</v>
       </c>
@@ -12277,7 +12340,7 @@
       </c>
       <c r="J59" s="26"/>
     </row>
-    <row r="60" spans="1:10">
+    <row r="60" spans="1:10" ht="14">
       <c r="A60" s="24" t="s">
         <v>145</v>
       </c>
@@ -12301,7 +12364,7 @@
       </c>
       <c r="J60" s="26"/>
     </row>
-    <row r="61" spans="1:10" ht="25.5">
+    <row r="61" spans="1:10" ht="28">
       <c r="A61" s="24" t="s">
         <v>147</v>
       </c>
@@ -12466,20 +12529,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AMJ100"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" customWidth="1"/>
-    <col min="3" max="3" width="12.28515625" customWidth="1"/>
-    <col min="4" max="4" width="51.85546875" customWidth="1"/>
-    <col min="5" max="5" width="17.7109375" customWidth="1"/>
-    <col min="6" max="6" width="51.85546875" customWidth="1"/>
+    <col min="1" max="1" width="10.33203125" customWidth="1"/>
+    <col min="3" max="3" width="12.33203125" customWidth="1"/>
+    <col min="4" max="4" width="51.83203125" customWidth="1"/>
+    <col min="5" max="5" width="17.6640625" customWidth="1"/>
+    <col min="6" max="6" width="51.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1024" s="29" customFormat="1" ht="18">
@@ -12487,7 +12550,8 @@
         <v>8</v>
       </c>
       <c r="B1" s="34">
-        <v>1</v>
+        <f>'Sprint 02 Backlog'!B1+1</f>
+        <v>3</v>
       </c>
       <c r="C1" s="34"/>
       <c r="D1" s="28" t="s">
@@ -12503,7 +12567,8 @@
         <v>150</v>
       </c>
       <c r="B2" s="30">
-        <v>44474</v>
+        <f>'Sprint 02 Backlog'!B3</f>
+        <v>44488</v>
       </c>
       <c r="C2" s="34"/>
       <c r="D2" s="31" t="s">
@@ -12520,7 +12585,7 @@
       </c>
       <c r="B3" s="30">
         <f>B2+7</f>
-        <v>44481</v>
+        <v>44495</v>
       </c>
       <c r="C3" s="34"/>
       <c r="D3" s="34"/>
@@ -12573,7 +12638,7 @@
       </c>
       <c r="B7" s="34">
         <f>COUNTA(D17:D995)</f>
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="C7" s="34"/>
       <c r="D7" s="34"/>
@@ -12588,11 +12653,11 @@
       </c>
       <c r="B8" s="34">
         <f t="shared" ref="B8:B14" si="0">B7-C8</f>
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C8" s="34">
         <f>COUNTIF(E$17:E$995, "Completed Day 1")</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D8" s="34"/>
       <c r="E8" s="34"/>
@@ -12606,7 +12671,7 @@
       </c>
       <c r="B9" s="34">
         <f t="shared" si="0"/>
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C9" s="34">
         <f>COUNTIF(E$17:E$995, "Completed Day 2")</f>
@@ -12624,7 +12689,7 @@
       </c>
       <c r="B10" s="34">
         <f t="shared" si="0"/>
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C10" s="34">
         <f>COUNTIF(E$17:E$995, "Completed Day 3")</f>
@@ -12642,7 +12707,7 @@
       </c>
       <c r="B11" s="34">
         <f t="shared" si="0"/>
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C11" s="34">
         <f>COUNTIF(E$17:E$995, "Completed Day 4")</f>
@@ -12660,11 +12725,11 @@
       </c>
       <c r="B12" s="34">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="C12" s="34">
         <f>COUNTIF(E$17:E$995, "Completed Day 5")</f>
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="D12" s="34"/>
       <c r="E12" s="34"/>
@@ -12678,11 +12743,11 @@
       </c>
       <c r="B13" s="34">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="C13" s="34">
         <f>COUNTIF(E$17:E$995, "Completed Day 6")</f>
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D13" s="34"/>
       <c r="E13" s="34"/>
@@ -12696,7 +12761,7 @@
       </c>
       <c r="B14" s="34">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="C14" s="34">
         <f>COUNTIF(E$17:E$995, "Completed Day 7")</f>
@@ -13761,16 +13826,16 @@
         <v>1</v>
       </c>
       <c r="B17" s="36" t="s">
-        <v>30</v>
+        <v>47</v>
       </c>
       <c r="C17" s="37" t="s">
         <v>170</v>
       </c>
       <c r="D17" s="38" t="s">
-        <v>175</v>
+        <v>206</v>
       </c>
       <c r="E17" s="39" t="s">
-        <v>172</v>
+        <v>208</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -13778,50 +13843,46 @@
         <v>2</v>
       </c>
       <c r="B18" s="36" t="s">
-        <v>30</v>
+        <v>47</v>
       </c>
       <c r="C18" s="37" t="s">
         <v>170</v>
       </c>
       <c r="D18" s="36" t="s">
-        <v>176</v>
-      </c>
-      <c r="E18" s="39" t="s">
-        <v>172</v>
-      </c>
+        <v>207</v>
+      </c>
+      <c r="E18" s="39"/>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="37">
         <v>3</v>
       </c>
       <c r="B19" s="36" t="s">
-        <v>30</v>
+        <v>47</v>
       </c>
       <c r="C19" s="37" t="s">
         <v>170</v>
       </c>
       <c r="D19" s="36" t="s">
-        <v>177</v>
-      </c>
-      <c r="E19" s="39" t="s">
-        <v>172</v>
-      </c>
+        <v>209</v>
+      </c>
+      <c r="E19" s="39"/>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="37">
         <v>4</v>
       </c>
       <c r="B20" s="36" t="s">
-        <v>30</v>
+        <v>51</v>
       </c>
       <c r="C20" s="37" t="s">
         <v>170</v>
       </c>
       <c r="D20" s="36" t="s">
-        <v>178</v>
+        <v>210</v>
       </c>
       <c r="E20" s="39" t="s">
-        <v>172</v>
+        <v>208</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -13829,50 +13890,46 @@
         <v>5</v>
       </c>
       <c r="B21" s="36" t="s">
-        <v>30</v>
+        <v>51</v>
       </c>
       <c r="C21" s="37" t="s">
         <v>170</v>
       </c>
       <c r="D21" s="36" t="s">
-        <v>179</v>
-      </c>
-      <c r="E21" s="39" t="s">
-        <v>173</v>
-      </c>
+        <v>211</v>
+      </c>
+      <c r="E21" s="39"/>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="37">
         <v>6</v>
       </c>
       <c r="B22" s="36" t="s">
-        <v>34</v>
+        <v>51</v>
       </c>
       <c r="C22" s="37" t="s">
         <v>170</v>
       </c>
       <c r="D22" s="36" t="s">
-        <v>180</v>
-      </c>
-      <c r="E22" s="39" t="s">
-        <v>172</v>
-      </c>
+        <v>212</v>
+      </c>
+      <c r="E22" s="39"/>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="37">
         <v>7</v>
       </c>
       <c r="B23" s="36" t="s">
-        <v>34</v>
+        <v>61</v>
       </c>
       <c r="C23" s="37" t="s">
         <v>170</v>
       </c>
       <c r="D23" s="36" t="s">
-        <v>181</v>
+        <v>213</v>
       </c>
       <c r="E23" s="39" t="s">
-        <v>172</v>
+        <v>208</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -13880,50 +13937,46 @@
         <v>8</v>
       </c>
       <c r="B24" s="36" t="s">
-        <v>34</v>
+        <v>61</v>
       </c>
       <c r="C24" s="37" t="s">
         <v>170</v>
       </c>
       <c r="D24" s="36" t="s">
-        <v>182</v>
-      </c>
-      <c r="E24" s="39" t="s">
-        <v>172</v>
-      </c>
+        <v>214</v>
+      </c>
+      <c r="E24" s="39"/>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="37">
         <v>9</v>
       </c>
       <c r="B25" s="36" t="s">
-        <v>34</v>
+        <v>61</v>
       </c>
       <c r="C25" s="37" t="s">
         <v>170</v>
       </c>
       <c r="D25" s="36" t="s">
-        <v>179</v>
-      </c>
-      <c r="E25" s="39" t="s">
-        <v>173</v>
-      </c>
+        <v>215</v>
+      </c>
+      <c r="E25" s="39"/>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="37">
         <v>10</v>
       </c>
       <c r="B26" s="36" t="s">
-        <v>37</v>
+        <v>56</v>
       </c>
       <c r="C26" s="37" t="s">
         <v>170</v>
       </c>
       <c r="D26" s="36" t="s">
-        <v>183</v>
+        <v>216</v>
       </c>
       <c r="E26" s="39" t="s">
-        <v>173</v>
+        <v>208</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -13931,113 +13984,149 @@
         <v>11</v>
       </c>
       <c r="B27" s="36" t="s">
-        <v>37</v>
+        <v>56</v>
       </c>
       <c r="C27" s="37" t="s">
         <v>170</v>
       </c>
       <c r="D27" s="36" t="s">
-        <v>184</v>
-      </c>
-      <c r="E27" s="39" t="s">
-        <v>173</v>
-      </c>
+        <v>217</v>
+      </c>
+      <c r="E27" s="39"/>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="37">
         <v>12</v>
       </c>
       <c r="B28" s="36" t="s">
-        <v>37</v>
+        <v>56</v>
       </c>
       <c r="C28" s="37" t="s">
         <v>170</v>
       </c>
       <c r="D28" s="36" t="s">
-        <v>185</v>
-      </c>
-      <c r="E28" s="39" t="s">
-        <v>173</v>
-      </c>
+        <v>218</v>
+      </c>
+      <c r="E28" s="39"/>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="37">
         <v>13</v>
       </c>
       <c r="B29" s="36" t="s">
-        <v>37</v>
+        <v>51</v>
       </c>
       <c r="C29" s="37" t="s">
         <v>170</v>
       </c>
       <c r="D29" s="36" t="s">
-        <v>186</v>
-      </c>
-      <c r="E29" s="39" t="s">
-        <v>173</v>
-      </c>
+        <v>219</v>
+      </c>
+      <c r="E29" s="39"/>
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="37">
         <v>14</v>
       </c>
-      <c r="B30" s="36"/>
-      <c r="C30" s="37"/>
-      <c r="D30" s="36"/>
+      <c r="B30" s="36" t="s">
+        <v>54</v>
+      </c>
+      <c r="C30" s="37" t="s">
+        <v>170</v>
+      </c>
+      <c r="D30" s="36" t="s">
+        <v>220</v>
+      </c>
       <c r="E30" s="39"/>
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="37">
         <v>15</v>
       </c>
-      <c r="B31" s="36"/>
-      <c r="C31" s="37"/>
-      <c r="D31" s="36"/>
+      <c r="B31" s="36" t="s">
+        <v>51</v>
+      </c>
+      <c r="C31" s="37" t="s">
+        <v>170</v>
+      </c>
+      <c r="D31" s="36" t="s">
+        <v>221</v>
+      </c>
       <c r="E31" s="39"/>
     </row>
     <row r="32" spans="1:5">
       <c r="A32" s="37">
         <v>16</v>
       </c>
-      <c r="B32" s="36"/>
-      <c r="C32" s="37"/>
-      <c r="D32" s="36"/>
+      <c r="B32" s="36" t="s">
+        <v>54</v>
+      </c>
+      <c r="C32" s="37" t="s">
+        <v>170</v>
+      </c>
+      <c r="D32" s="36" t="s">
+        <v>226</v>
+      </c>
       <c r="E32" s="39"/>
     </row>
     <row r="33" spans="1:5">
       <c r="A33" s="37">
         <v>17</v>
       </c>
-      <c r="B33" s="36"/>
-      <c r="C33" s="37"/>
-      <c r="D33" s="36"/>
+      <c r="B33" s="36" t="s">
+        <v>51</v>
+      </c>
+      <c r="C33" s="37" t="s">
+        <v>170</v>
+      </c>
+      <c r="D33" s="36" t="s">
+        <v>222</v>
+      </c>
       <c r="E33" s="39"/>
     </row>
     <row r="34" spans="1:5">
       <c r="A34" s="37">
         <v>18</v>
       </c>
-      <c r="B34" s="36"/>
-      <c r="C34" s="37"/>
-      <c r="D34" s="36"/>
+      <c r="B34" s="36" t="s">
+        <v>54</v>
+      </c>
+      <c r="C34" s="37" t="s">
+        <v>170</v>
+      </c>
+      <c r="D34" s="36" t="s">
+        <v>223</v>
+      </c>
       <c r="E34" s="39"/>
     </row>
     <row r="35" spans="1:5">
       <c r="A35" s="37">
         <v>19</v>
       </c>
-      <c r="B35" s="36"/>
-      <c r="C35" s="37"/>
-      <c r="D35" s="36"/>
+      <c r="B35" s="36" t="s">
+        <v>51</v>
+      </c>
+      <c r="C35" s="37" t="s">
+        <v>170</v>
+      </c>
+      <c r="D35" s="36" t="s">
+        <v>224</v>
+      </c>
       <c r="E35" s="39"/>
     </row>
     <row r="36" spans="1:5">
       <c r="A36" s="37">
         <v>20</v>
       </c>
-      <c r="B36" s="36"/>
-      <c r="C36" s="37"/>
-      <c r="D36" s="36"/>
+      <c r="B36" s="36" t="s">
+        <v>54</v>
+      </c>
+      <c r="C36" s="37" t="s">
+        <v>170</v>
+      </c>
+      <c r="D36" s="36" t="s">
+        <v>225</v>
+      </c>
       <c r="E36" s="39"/>
     </row>
     <row r="37" spans="1:5">
@@ -14618,20 +14707,20 @@
     </row>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Task ID" prompt="This is just an arbitrary unique (per sprint) integer assigned to a task, used by the team to refer to that task. " sqref="A17:A100" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Task ID" prompt="This is just an arbitrary unique (per sprint) integer assigned to a task, used by the team to refer to that task. " sqref="A17:A100" xr:uid="{00000000-0002-0000-0300-000000000000}">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="OPTIONAL" prompt="You may add any notes here that help understand the requirements and scope for this task" sqref="F17:F100" xr:uid="{00000000-0002-0000-0100-000004000000}">
+    <dataValidation type="list" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Wrong Value" error="This cell may only contain a valid status value (hint: use the drop-down selection list) or be left blank (hint: use the Delete key)" promptTitle="Implementation Status" prompt="Leave blank until task is begun._x000a_Select &quot;In Work&quot; when started (for long tasks only)._x000a_Select Completed ONLY when this task is done._x000a_    Select &quot;Completed Day 1&quot; if finished on the first day, and_x000a_    similarly for &quot;Completed on Day 2&quot; et. al." sqref="E17:E100" xr:uid="{00000000-0002-0000-0300-000003000000}">
+      <formula1>"In Work,Completed Day 1,Completed Day 2,Completed Day 3,Completed Day 4,Completed Day 5,Completed Day 6,Completed Day 7,"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="OPTIONAL" prompt="You may add any notes here that help understand the requirements and scope for this task" sqref="F17:F100" xr:uid="{00000000-0002-0000-0300-000004000000}">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Task Description" prompt="Select a Feature ID to the left. Then, in this column, list each discrete task needed to implement that feature._x000a__x000a_Example tasks might be &quot;create the Foo class&quot;, &quot;add the Bar method to the (existing) Qux class&quot;, &quot;Find icons for the task bar&quot;, &quot;Update the m" sqref="D18:D22 D26:D29 D31:D100" xr:uid="{00000000-0002-0000-0100-000005000000}">
+    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Task Description" prompt="Select a Feature ID to the left. Then, in this column, list each discrete task needed to implement that feature._x000a__x000a_Example tasks might be &quot;create the Foo class&quot;, &quot;add the Bar method to the (existing) Qux class&quot;, &quot;Find icons for the task bar&quot;, &quot;Update the m" sqref="D18:D28 D30:D100" xr:uid="{00000000-0002-0000-0300-000005000000}">
       <formula1>0</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation type="list" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Wrong Value" error="This cell may only contain a valid status value (hint: use the drop-down selection list) or be left blank (hint: use the Delete key)" promptTitle="Implementation Status" prompt="Leave blank until task is begun._x000a_Select &quot;In Work&quot; when started (for long tasks only)._x000a_Select Completed ONLY when this task is done._x000a_    Select &quot;Completed Day 1&quot; if finished on the first day, and_x000a_    similarly for &quot;Completed on Day 2&quot; et. al." sqref="E17:E29 E31:E100" xr:uid="{00000000-0002-0000-0100-000003000000}">
-      <formula1>"In Work,Completed Day 1,Completed Day 2,Completed Day 3,Completed Day 4,Completed Day 5,Completed Day 6,Completed Day 7,"</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
@@ -14645,23 +14734,23 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
-        <x14:dataValidation type="list" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Select Feature ID from Product Backlog" prompt="The list contains the Feature IDs from the same column on the Product Backlog tab._x000a__x000a_For each (ahem) Feature ID, create one or more rows in this table representing the tasks you need to complete to implement that feature._x000a__x000a_For example, for a &quot;Provide Help " xr:uid="{00000000-0002-0000-0100-000001000000}">
+        <x14:dataValidation type="list" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Select Feature ID from Product Backlog" prompt="The list contains the Feature IDs from the same column on the Product Backlog tab._x000a__x000a_For each (ahem) Feature ID, create one or more rows in this table representing the tasks you need to complete to implement that feature._x000a__x000a_For example, for a &quot;Provide Help " xr:uid="{00000000-0002-0000-0300-000001000000}">
           <x14:formula1>
             <xm:f>'Product Backlog'!$A$24:$A$66</xm:f>
           </x14:formula1>
           <x14:formula2>
             <xm:f>0</xm:f>
           </x14:formula2>
-          <xm:sqref>B17:B29 B31:B100</xm:sqref>
+          <xm:sqref>B17:B100</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Select Feature ID from Product Backlog" prompt="Exactly ONE team member may be responsible for any task, and they will receive grade credit for their work._x000a__x000a_If you have more than one person on your team, each member MUST select their initials for each task the agree to perform. Use this to ensure that " xr:uid="{00000000-0002-0000-0100-000002000000}">
+        <x14:dataValidation type="list" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Select Feature ID from Product Backlog" prompt="Exactly ONE team member may be responsible for any task, and they will receive grade credit for their work._x000a__x000a_If you have more than one person on your team, each member MUST select their initials for each task the agree to perform. Use this to ensure that " xr:uid="{00000000-0002-0000-0300-000002000000}">
           <x14:formula1>
             <xm:f>'Product Backlog'!$G$5:$G$8</xm:f>
           </x14:formula1>
           <x14:formula2>
             <xm:f>0</xm:f>
           </x14:formula2>
-          <xm:sqref>C17:C29 C31:C100</xm:sqref>
+          <xm:sqref>C17:C100</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -14670,20 +14759,20 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AMJ100"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+    <sheetView topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" customWidth="1"/>
-    <col min="3" max="3" width="12.28515625" customWidth="1"/>
-    <col min="4" max="4" width="51.85546875" customWidth="1"/>
-    <col min="5" max="5" width="17.7109375" customWidth="1"/>
-    <col min="6" max="6" width="51.85546875" customWidth="1"/>
+    <col min="1" max="1" width="10.33203125" customWidth="1"/>
+    <col min="3" max="3" width="12.33203125" customWidth="1"/>
+    <col min="4" max="4" width="51.83203125" customWidth="1"/>
+    <col min="5" max="5" width="17.6640625" customWidth="1"/>
+    <col min="6" max="6" width="51.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1024" s="29" customFormat="1" ht="18">
@@ -14691,8 +14780,7 @@
         <v>8</v>
       </c>
       <c r="B1" s="34">
-        <f>'Sprint 01 Backlog'!B1+1</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C1" s="34"/>
       <c r="D1" s="28" t="s">
@@ -14708,8 +14796,7 @@
         <v>150</v>
       </c>
       <c r="B2" s="30">
-        <f>'Sprint 01 Backlog'!B3</f>
-        <v>44481</v>
+        <v>44474</v>
       </c>
       <c r="C2" s="34"/>
       <c r="D2" s="31" t="s">
@@ -14726,7 +14813,7 @@
       </c>
       <c r="B3" s="30">
         <f>B2+7</f>
-        <v>44488</v>
+        <v>44481</v>
       </c>
       <c r="C3" s="34"/>
       <c r="D3" s="34"/>
@@ -14779,7 +14866,7 @@
       </c>
       <c r="B7" s="34">
         <f>COUNTA(D17:D995)</f>
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C7" s="34"/>
       <c r="D7" s="34"/>
@@ -14794,7 +14881,7 @@
       </c>
       <c r="B8" s="34">
         <f t="shared" ref="B8:B14" si="0">B7-C8</f>
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C8" s="34">
         <f>COUNTIF(E$17:E$995, "Completed Day 1")</f>
@@ -14812,11 +14899,11 @@
       </c>
       <c r="B9" s="34">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C9" s="34">
         <f>COUNTIF(E$17:E$995, "Completed Day 2")</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D9" s="34"/>
       <c r="E9" s="34"/>
@@ -14830,11 +14917,11 @@
       </c>
       <c r="B10" s="34">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="C10" s="34">
         <f>COUNTIF(E$17:E$995, "Completed Day 3")</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D10" s="34"/>
       <c r="E10" s="34"/>
@@ -14848,11 +14935,11 @@
       </c>
       <c r="B11" s="34">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="C11" s="34">
         <f>COUNTIF(E$17:E$995, "Completed Day 4")</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D11" s="34"/>
       <c r="E11" s="34"/>
@@ -14866,11 +14953,11 @@
       </c>
       <c r="B12" s="34">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C12" s="34">
         <f>COUNTIF(E$17:E$995, "Completed Day 5")</f>
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="D12" s="34"/>
       <c r="E12" s="34"/>
@@ -14888,7 +14975,7 @@
       </c>
       <c r="C13" s="34">
         <f>COUNTIF(E$17:E$995, "Completed Day 6")</f>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D13" s="34"/>
       <c r="E13" s="34"/>
@@ -15962,232 +16049,228 @@
       <c r="AMI16" s="37"/>
       <c r="AMJ16" s="37"/>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:5">
       <c r="A17" s="37">
         <v>1</v>
       </c>
       <c r="B17" s="36" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="C17" s="37" t="s">
         <v>170</v>
       </c>
-      <c r="D17" s="36" t="s">
-        <v>187</v>
+      <c r="D17" s="38" t="s">
+        <v>175</v>
       </c>
       <c r="E17" s="39" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
       <c r="A18" s="37">
         <v>2</v>
       </c>
       <c r="B18" s="36" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="C18" s="37" t="s">
         <v>170</v>
       </c>
       <c r="D18" s="36" t="s">
-        <v>189</v>
+        <v>176</v>
       </c>
       <c r="E18" s="39" t="s">
-        <v>190</v>
-      </c>
-      <c r="F18" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
       <c r="A19" s="37">
         <v>3</v>
       </c>
       <c r="B19" s="36" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="C19" s="37" t="s">
         <v>170</v>
       </c>
       <c r="D19" s="36" t="s">
-        <v>196</v>
+        <v>177</v>
       </c>
       <c r="E19" s="39" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
       <c r="A20" s="37">
         <v>4</v>
       </c>
       <c r="B20" s="36" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="C20" s="37" t="s">
         <v>170</v>
       </c>
       <c r="D20" s="36" t="s">
-        <v>191</v>
+        <v>178</v>
       </c>
       <c r="E20" s="39" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
       <c r="A21" s="37">
         <v>5</v>
       </c>
       <c r="B21" s="36" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="C21" s="37" t="s">
         <v>170</v>
       </c>
       <c r="D21" s="36" t="s">
-        <v>192</v>
+        <v>179</v>
       </c>
       <c r="E21" s="39" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
       <c r="A22" s="37">
         <v>6</v>
       </c>
       <c r="B22" s="36" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C22" s="37" t="s">
         <v>170</v>
       </c>
       <c r="D22" s="36" t="s">
-        <v>193</v>
+        <v>180</v>
       </c>
       <c r="E22" s="39" t="s">
-        <v>188</v>
-      </c>
-      <c r="F22" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
       <c r="A23" s="37">
         <v>7</v>
       </c>
       <c r="B23" s="36" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C23" s="37" t="s">
         <v>170</v>
       </c>
       <c r="D23" s="36" t="s">
-        <v>194</v>
+        <v>181</v>
       </c>
       <c r="E23" s="39" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
       <c r="A24" s="37">
         <v>8</v>
       </c>
       <c r="B24" s="36" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="C24" s="37" t="s">
         <v>170</v>
       </c>
       <c r="D24" s="36" t="s">
-        <v>199</v>
+        <v>182</v>
       </c>
       <c r="E24" s="39" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
       <c r="A25" s="37">
         <v>9</v>
       </c>
       <c r="B25" s="36" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="C25" s="37" t="s">
         <v>170</v>
       </c>
       <c r="D25" s="36" t="s">
-        <v>200</v>
+        <v>179</v>
       </c>
       <c r="E25" s="39" t="s">
-        <v>172</v>
-      </c>
-      <c r="F25" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
       <c r="A26" s="37">
         <v>10</v>
       </c>
       <c r="B26" s="36" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C26" s="37" t="s">
         <v>170</v>
       </c>
       <c r="D26" s="36" t="s">
-        <v>202</v>
+        <v>183</v>
       </c>
       <c r="E26" s="39" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:5">
       <c r="A27" s="37">
         <v>11</v>
       </c>
       <c r="B27" s="36" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="C27" s="37" t="s">
         <v>170</v>
       </c>
       <c r="D27" s="36" t="s">
-        <v>203</v>
+        <v>184</v>
       </c>
       <c r="E27" s="39" t="s">
-        <v>172</v>
-      </c>
-      <c r="F27" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
       <c r="A28" s="37">
         <v>12</v>
       </c>
       <c r="B28" s="36" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="C28" s="37" t="s">
         <v>170</v>
       </c>
       <c r="D28" s="36" t="s">
-        <v>205</v>
+        <v>185</v>
       </c>
       <c r="E28" s="39" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:5">
       <c r="A29" s="37">
         <v>13</v>
       </c>
-      <c r="B29" s="36"/>
-      <c r="C29" s="37"/>
-      <c r="D29" s="36"/>
-      <c r="E29" s="39"/>
-    </row>
-    <row r="30" spans="1:6">
+      <c r="B29" s="36" t="s">
+        <v>37</v>
+      </c>
+      <c r="C29" s="37" t="s">
+        <v>170</v>
+      </c>
+      <c r="D29" s="36" t="s">
+        <v>186</v>
+      </c>
+      <c r="E29" s="39" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
       <c r="A30" s="37">
         <v>14</v>
       </c>
@@ -16196,7 +16279,7 @@
       <c r="D30" s="36"/>
       <c r="E30" s="39"/>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31" spans="1:5">
       <c r="A31" s="37">
         <v>15</v>
       </c>
@@ -16205,7 +16288,7 @@
       <c r="D31" s="36"/>
       <c r="E31" s="39"/>
     </row>
-    <row r="32" spans="1:6">
+    <row r="32" spans="1:5">
       <c r="A32" s="37">
         <v>16</v>
       </c>
@@ -16827,22 +16910,21 @@
       <c r="E100" s="39"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="11" type="noConversion"/>
   <dataValidations count="4">
-    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Task ID" prompt="This is just an arbitrary unique (per sprint) integer assigned to a task, used by the team to refer to that task. " sqref="A17:A100" xr:uid="{00000000-0002-0000-0200-000000000000}">
+    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Task ID" prompt="This is just an arbitrary unique (per sprint) integer assigned to a task, used by the team to refer to that task. " sqref="A17:A100" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Wrong Value" error="This cell may only contain a valid status value (hint: use the drop-down selection list) or be left blank (hint: use the Delete key)" promptTitle="Implementation Status" prompt="Leave blank until task is begun._x000a_Select &quot;In Work&quot; when started (for long tasks only)._x000a_Select Completed ONLY when this task is done._x000a_    Select &quot;Completed Day 1&quot; if finished on the first day, and_x000a_    similarly for &quot;Completed on Day 2&quot; et. al." sqref="E17:E100" xr:uid="{00000000-0002-0000-0200-000003000000}">
-      <formula1>"In Work,Completed Day 1,Completed Day 2,Completed Day 3,Completed Day 4,Completed Day 5,Completed Day 6,Completed Day 7,"</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Task Description" prompt="Select a Feature ID to the left. Then, in this column, list each discrete task needed to implement that feature._x000a__x000a_Example tasks might be &quot;create the Foo class&quot;, &quot;add the Bar method to the (existing) Qux class&quot;, &quot;Find icons for the task bar&quot;, &quot;Update the m" sqref="D29:D100 D17:D27" xr:uid="{00000000-0002-0000-0200-000005000000}">
+    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="OPTIONAL" prompt="You may add any notes here that help understand the requirements and scope for this task" sqref="F17:F100" xr:uid="{00000000-0002-0000-0100-000004000000}">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="OPTIONAL" prompt="You may add any notes here that help understand the requirements and scope for this task" sqref="F29:F100 F17:F27" xr:uid="{00000000-0002-0000-0200-000004000000}">
+    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Task Description" prompt="Select a Feature ID to the left. Then, in this column, list each discrete task needed to implement that feature._x000a__x000a_Example tasks might be &quot;create the Foo class&quot;, &quot;add the Bar method to the (existing) Qux class&quot;, &quot;Find icons for the task bar&quot;, &quot;Update the m" sqref="D18:D22 D26:D29 D38:D100" xr:uid="{00000000-0002-0000-0100-000005000000}">
       <formula1>0</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation type="list" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Wrong Value" error="This cell may only contain a valid status value (hint: use the drop-down selection list) or be left blank (hint: use the Delete key)" promptTitle="Implementation Status" prompt="Leave blank until task is begun._x000a_Select &quot;In Work&quot; when started (for long tasks only)._x000a_Select Completed ONLY when this task is done._x000a_    Select &quot;Completed Day 1&quot; if finished on the first day, and_x000a_    similarly for &quot;Completed on Day 2&quot; et. al." sqref="E17:E29 E31:E100" xr:uid="{00000000-0002-0000-0100-000003000000}">
+      <formula1>"In Work,Completed Day 1,Completed Day 2,Completed Day 3,Completed Day 4,Completed Day 5,Completed Day 6,Completed Day 7,"</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
@@ -16856,23 +16938,23 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
-        <x14:dataValidation type="list" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Select Feature ID from Product Backlog" prompt="The list contains the Feature IDs from the same column on the Product Backlog tab._x000a__x000a_For each (ahem) Feature ID, create one or more rows in this table representing the tasks you need to complete to implement that feature._x000a__x000a_For example, for a &quot;Provide Help " xr:uid="{00000000-0002-0000-0200-000001000000}">
+        <x14:dataValidation type="list" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Select Feature ID from Product Backlog" prompt="The list contains the Feature IDs from the same column on the Product Backlog tab._x000a__x000a_For each (ahem) Feature ID, create one or more rows in this table representing the tasks you need to complete to implement that feature._x000a__x000a_For example, for a &quot;Provide Help " xr:uid="{00000000-0002-0000-0100-000001000000}">
           <x14:formula1>
             <xm:f>'Product Backlog'!$A$24:$A$66</xm:f>
           </x14:formula1>
           <x14:formula2>
             <xm:f>0</xm:f>
           </x14:formula2>
-          <xm:sqref>B29:B100 B17:B27</xm:sqref>
+          <xm:sqref>B17:B29 B31:B100</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Select Feature ID from Product Backlog" prompt="Exactly ONE team member may be responsible for any task, and they will receive grade credit for their work._x000a__x000a_If you have more than one person on your team, each member MUST select their initials for each task the agree to perform. Use this to ensure that " xr:uid="{00000000-0002-0000-0200-000002000000}">
+        <x14:dataValidation type="list" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Select Feature ID from Product Backlog" prompt="Exactly ONE team member may be responsible for any task, and they will receive grade credit for their work._x000a__x000a_If you have more than one person on your team, each member MUST select their initials for each task the agree to perform. Use this to ensure that " xr:uid="{00000000-0002-0000-0100-000002000000}">
           <x14:formula1>
             <xm:f>'Product Backlog'!$G$5:$G$8</xm:f>
           </x14:formula1>
           <x14:formula2>
             <xm:f>0</xm:f>
           </x14:formula2>
-          <xm:sqref>C29:C100 C17:C27</xm:sqref>
+          <xm:sqref>C17:C29 C31:C100</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -16881,20 +16963,20 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AMJ100"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" customWidth="1"/>
-    <col min="3" max="3" width="12.28515625" customWidth="1"/>
-    <col min="4" max="4" width="51.85546875" customWidth="1"/>
-    <col min="5" max="5" width="17.7109375" customWidth="1"/>
-    <col min="6" max="6" width="51.85546875" customWidth="1"/>
+    <col min="1" max="1" width="10.33203125" customWidth="1"/>
+    <col min="3" max="3" width="12.33203125" customWidth="1"/>
+    <col min="4" max="4" width="51.83203125" customWidth="1"/>
+    <col min="5" max="5" width="17.6640625" customWidth="1"/>
+    <col min="6" max="6" width="51.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1024" s="29" customFormat="1" ht="18">
@@ -16902,8 +16984,8 @@
         <v>8</v>
       </c>
       <c r="B1" s="34">
-        <f>'Sprint 02 Backlog'!B1+1</f>
-        <v>3</v>
+        <f>'Sprint 01 Backlog'!B1+1</f>
+        <v>2</v>
       </c>
       <c r="C1" s="34"/>
       <c r="D1" s="28" t="s">
@@ -16919,8 +17001,8 @@
         <v>150</v>
       </c>
       <c r="B2" s="30">
-        <f>'Sprint 02 Backlog'!B3</f>
-        <v>44488</v>
+        <f>'Sprint 01 Backlog'!B3</f>
+        <v>44481</v>
       </c>
       <c r="C2" s="34"/>
       <c r="D2" s="31" t="s">
@@ -16937,7 +17019,7 @@
       </c>
       <c r="B3" s="30">
         <f>B2+7</f>
-        <v>44495</v>
+        <v>44488</v>
       </c>
       <c r="C3" s="34"/>
       <c r="D3" s="34"/>
@@ -16990,7 +17072,7 @@
       </c>
       <c r="B7" s="34">
         <f>COUNTA(D17:D995)</f>
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="C7" s="34"/>
       <c r="D7" s="34"/>
@@ -17005,7 +17087,7 @@
       </c>
       <c r="B8" s="34">
         <f t="shared" ref="B8:B14" si="0">B7-C8</f>
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="C8" s="34">
         <f>COUNTIF(E$17:E$995, "Completed Day 1")</f>
@@ -17023,11 +17105,11 @@
       </c>
       <c r="B9" s="34">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="C9" s="34">
         <f>COUNTIF(E$17:E$995, "Completed Day 2")</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D9" s="34"/>
       <c r="E9" s="34"/>
@@ -17041,11 +17123,11 @@
       </c>
       <c r="B10" s="34">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C10" s="34">
         <f>COUNTIF(E$17:E$995, "Completed Day 3")</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D10" s="34"/>
       <c r="E10" s="34"/>
@@ -17059,11 +17141,11 @@
       </c>
       <c r="B11" s="34">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C11" s="34">
         <f>COUNTIF(E$17:E$995, "Completed Day 4")</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D11" s="34"/>
       <c r="E11" s="34"/>
@@ -17077,11 +17159,11 @@
       </c>
       <c r="B12" s="34">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C12" s="34">
         <f>COUNTIF(E$17:E$995, "Completed Day 5")</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D12" s="34"/>
       <c r="E12" s="34"/>
@@ -17095,11 +17177,11 @@
       </c>
       <c r="B13" s="34">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C13" s="34">
         <f>COUNTIF(E$17:E$995, "Completed Day 6")</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D13" s="34"/>
       <c r="E13" s="34"/>
@@ -17113,7 +17195,7 @@
       </c>
       <c r="B14" s="34">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C14" s="34">
         <f>COUNTIF(E$17:E$995, "Completed Day 7")</f>
@@ -18173,117 +18255,223 @@
       <c r="AMI16" s="37"/>
       <c r="AMJ16" s="37"/>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:6">
       <c r="A17" s="37">
         <v>1</v>
       </c>
-      <c r="B17" s="36"/>
-      <c r="C17" s="37"/>
-      <c r="D17" s="38" t="s">
-        <v>167</v>
-      </c>
-      <c r="E17" s="39"/>
-    </row>
-    <row r="18" spans="1:5">
+      <c r="B17" s="36" t="s">
+        <v>40</v>
+      </c>
+      <c r="C17" s="37" t="s">
+        <v>170</v>
+      </c>
+      <c r="D17" s="36" t="s">
+        <v>187</v>
+      </c>
+      <c r="E17" s="39" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
       <c r="A18" s="37">
         <v>2</v>
       </c>
-      <c r="B18" s="36"/>
-      <c r="C18" s="37"/>
-      <c r="D18" s="36"/>
-      <c r="E18" s="39"/>
-    </row>
-    <row r="19" spans="1:5">
+      <c r="B18" s="36" t="s">
+        <v>40</v>
+      </c>
+      <c r="C18" s="37" t="s">
+        <v>170</v>
+      </c>
+      <c r="D18" s="36" t="s">
+        <v>189</v>
+      </c>
+      <c r="E18" s="39" t="s">
+        <v>190</v>
+      </c>
+      <c r="F18" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
       <c r="A19" s="37">
         <v>3</v>
       </c>
-      <c r="B19" s="36"/>
-      <c r="C19" s="37"/>
-      <c r="D19" s="36"/>
-      <c r="E19" s="39"/>
-    </row>
-    <row r="20" spans="1:5">
+      <c r="B19" s="36" t="s">
+        <v>40</v>
+      </c>
+      <c r="C19" s="37" t="s">
+        <v>170</v>
+      </c>
+      <c r="D19" s="36" t="s">
+        <v>196</v>
+      </c>
+      <c r="E19" s="39" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
       <c r="A20" s="37">
         <v>4</v>
       </c>
-      <c r="B20" s="36"/>
-      <c r="C20" s="37"/>
-      <c r="D20" s="36"/>
-      <c r="E20" s="39"/>
-    </row>
-    <row r="21" spans="1:5">
+      <c r="B20" s="36" t="s">
+        <v>40</v>
+      </c>
+      <c r="C20" s="37" t="s">
+        <v>170</v>
+      </c>
+      <c r="D20" s="36" t="s">
+        <v>191</v>
+      </c>
+      <c r="E20" s="39" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
       <c r="A21" s="37">
         <v>5</v>
       </c>
-      <c r="B21" s="36"/>
-      <c r="C21" s="37"/>
-      <c r="D21" s="36"/>
-      <c r="E21" s="39"/>
-    </row>
-    <row r="22" spans="1:5">
+      <c r="B21" s="36" t="s">
+        <v>40</v>
+      </c>
+      <c r="C21" s="37" t="s">
+        <v>170</v>
+      </c>
+      <c r="D21" s="36" t="s">
+        <v>192</v>
+      </c>
+      <c r="E21" s="39" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
       <c r="A22" s="37">
         <v>6</v>
       </c>
-      <c r="B22" s="36"/>
-      <c r="C22" s="37"/>
-      <c r="D22" s="36"/>
-      <c r="E22" s="39"/>
-    </row>
-    <row r="23" spans="1:5">
+      <c r="B22" s="36" t="s">
+        <v>40</v>
+      </c>
+      <c r="C22" s="37" t="s">
+        <v>170</v>
+      </c>
+      <c r="D22" s="36" t="s">
+        <v>193</v>
+      </c>
+      <c r="E22" s="39" t="s">
+        <v>188</v>
+      </c>
+      <c r="F22" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
       <c r="A23" s="37">
         <v>7</v>
       </c>
-      <c r="B23" s="36"/>
-      <c r="C23" s="37"/>
-      <c r="D23" s="36"/>
-      <c r="E23" s="39"/>
-    </row>
-    <row r="24" spans="1:5">
+      <c r="B23" s="36" t="s">
+        <v>40</v>
+      </c>
+      <c r="C23" s="37" t="s">
+        <v>170</v>
+      </c>
+      <c r="D23" s="36" t="s">
+        <v>194</v>
+      </c>
+      <c r="E23" s="39" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
       <c r="A24" s="37">
         <v>8</v>
       </c>
-      <c r="B24" s="36"/>
-      <c r="C24" s="37"/>
-      <c r="D24" s="36"/>
-      <c r="E24" s="39"/>
-    </row>
-    <row r="25" spans="1:5">
+      <c r="B24" s="36" t="s">
+        <v>44</v>
+      </c>
+      <c r="C24" s="37" t="s">
+        <v>170</v>
+      </c>
+      <c r="D24" s="36" t="s">
+        <v>199</v>
+      </c>
+      <c r="E24" s="39" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
       <c r="A25" s="37">
         <v>9</v>
       </c>
-      <c r="B25" s="36"/>
-      <c r="C25" s="37"/>
-      <c r="D25" s="36"/>
-      <c r="E25" s="39"/>
-    </row>
-    <row r="26" spans="1:5">
+      <c r="B25" s="36" t="s">
+        <v>44</v>
+      </c>
+      <c r="C25" s="37" t="s">
+        <v>170</v>
+      </c>
+      <c r="D25" s="36" t="s">
+        <v>200</v>
+      </c>
+      <c r="E25" s="39" t="s">
+        <v>172</v>
+      </c>
+      <c r="F25" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
       <c r="A26" s="37">
         <v>10</v>
       </c>
-      <c r="B26" s="36"/>
-      <c r="C26" s="37"/>
-      <c r="D26" s="36"/>
-      <c r="E26" s="39"/>
-    </row>
-    <row r="27" spans="1:5">
+      <c r="B26" s="36" t="s">
+        <v>40</v>
+      </c>
+      <c r="C26" s="37" t="s">
+        <v>170</v>
+      </c>
+      <c r="D26" s="36" t="s">
+        <v>202</v>
+      </c>
+      <c r="E26" s="39" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
       <c r="A27" s="37">
         <v>11</v>
       </c>
-      <c r="B27" s="36"/>
-      <c r="C27" s="37"/>
-      <c r="D27" s="36"/>
-      <c r="E27" s="39"/>
-    </row>
-    <row r="28" spans="1:5">
+      <c r="B27" s="36" t="s">
+        <v>44</v>
+      </c>
+      <c r="C27" s="37" t="s">
+        <v>170</v>
+      </c>
+      <c r="D27" s="36" t="s">
+        <v>203</v>
+      </c>
+      <c r="E27" s="39" t="s">
+        <v>172</v>
+      </c>
+      <c r="F27" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
       <c r="A28" s="37">
         <v>12</v>
       </c>
-      <c r="B28" s="36"/>
-      <c r="C28" s="37"/>
-      <c r="D28" s="36"/>
-      <c r="E28" s="39"/>
-    </row>
-    <row r="29" spans="1:5">
+      <c r="B28" s="36" t="s">
+        <v>44</v>
+      </c>
+      <c r="C28" s="37" t="s">
+        <v>170</v>
+      </c>
+      <c r="D28" s="36" t="s">
+        <v>205</v>
+      </c>
+      <c r="E28" s="39" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
       <c r="A29" s="37">
         <v>13</v>
       </c>
@@ -18292,7 +18480,7 @@
       <c r="D29" s="36"/>
       <c r="E29" s="39"/>
     </row>
-    <row r="30" spans="1:5">
+    <row r="30" spans="1:6">
       <c r="A30" s="37">
         <v>14</v>
       </c>
@@ -18301,7 +18489,7 @@
       <c r="D30" s="36"/>
       <c r="E30" s="39"/>
     </row>
-    <row r="31" spans="1:5">
+    <row r="31" spans="1:6">
       <c r="A31" s="37">
         <v>15</v>
       </c>
@@ -18310,7 +18498,7 @@
       <c r="D31" s="36"/>
       <c r="E31" s="39"/>
     </row>
-    <row r="32" spans="1:5">
+    <row r="32" spans="1:6">
       <c r="A32" s="37">
         <v>16</v>
       </c>
@@ -18932,20 +19120,21 @@
       <c r="E100" s="39"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="11" type="noConversion"/>
   <dataValidations count="4">
-    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Task ID" prompt="This is just an arbitrary unique (per sprint) integer assigned to a task, used by the team to refer to that task. " sqref="A17:A100" xr:uid="{00000000-0002-0000-0300-000000000000}">
+    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Task ID" prompt="This is just an arbitrary unique (per sprint) integer assigned to a task, used by the team to refer to that task. " sqref="A17:A100" xr:uid="{00000000-0002-0000-0200-000000000000}">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Wrong Value" error="This cell may only contain a valid status value (hint: use the drop-down selection list) or be left blank (hint: use the Delete key)" promptTitle="Implementation Status" prompt="Leave blank until task is begun._x000a_Select &quot;In Work&quot; when started (for long tasks only)._x000a_Select Completed ONLY when this task is done._x000a_    Select &quot;Completed Day 1&quot; if finished on the first day, and_x000a_    similarly for &quot;Completed on Day 2&quot; et. al." sqref="E17:E100" xr:uid="{00000000-0002-0000-0300-000003000000}">
+    <dataValidation type="list" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Wrong Value" error="This cell may only contain a valid status value (hint: use the drop-down selection list) or be left blank (hint: use the Delete key)" promptTitle="Implementation Status" prompt="Leave blank until task is begun._x000a_Select &quot;In Work&quot; when started (for long tasks only)._x000a_Select Completed ONLY when this task is done._x000a_    Select &quot;Completed Day 1&quot; if finished on the first day, and_x000a_    similarly for &quot;Completed on Day 2&quot; et. al." sqref="E17:E100" xr:uid="{00000000-0002-0000-0200-000003000000}">
       <formula1>"In Work,Completed Day 1,Completed Day 2,Completed Day 3,Completed Day 4,Completed Day 5,Completed Day 6,Completed Day 7,"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="OPTIONAL" prompt="You may add any notes here that help understand the requirements and scope for this task" sqref="F17:F100" xr:uid="{00000000-0002-0000-0300-000004000000}">
+    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Task Description" prompt="Select a Feature ID to the left. Then, in this column, list each discrete task needed to implement that feature._x000a__x000a_Example tasks might be &quot;create the Foo class&quot;, &quot;add the Bar method to the (existing) Qux class&quot;, &quot;Find icons for the task bar&quot;, &quot;Update the m" sqref="D29:D100 D17:D27" xr:uid="{00000000-0002-0000-0200-000005000000}">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Task Description" prompt="Select a Feature ID to the left. Then, in this column, list each discrete task needed to implement that feature._x000a__x000a_Example tasks might be &quot;create the Foo class&quot;, &quot;add the Bar method to the (existing) Qux class&quot;, &quot;Find icons for the task bar&quot;, &quot;Update the m" sqref="D18:D100" xr:uid="{00000000-0002-0000-0300-000005000000}">
+    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="OPTIONAL" prompt="You may add any notes here that help understand the requirements and scope for this task" sqref="F29:F100 F17:F27" xr:uid="{00000000-0002-0000-0200-000004000000}">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -18960,23 +19149,23 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
-        <x14:dataValidation type="list" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Select Feature ID from Product Backlog" prompt="The list contains the Feature IDs from the same column on the Product Backlog tab._x000a__x000a_For each (ahem) Feature ID, create one or more rows in this table representing the tasks you need to complete to implement that feature._x000a__x000a_For example, for a &quot;Provide Help " xr:uid="{00000000-0002-0000-0300-000001000000}">
+        <x14:dataValidation type="list" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Select Feature ID from Product Backlog" prompt="The list contains the Feature IDs from the same column on the Product Backlog tab._x000a__x000a_For each (ahem) Feature ID, create one or more rows in this table representing the tasks you need to complete to implement that feature._x000a__x000a_For example, for a &quot;Provide Help " xr:uid="{00000000-0002-0000-0200-000001000000}">
           <x14:formula1>
             <xm:f>'Product Backlog'!$A$24:$A$66</xm:f>
           </x14:formula1>
           <x14:formula2>
             <xm:f>0</xm:f>
           </x14:formula2>
-          <xm:sqref>B17:B100</xm:sqref>
+          <xm:sqref>B29:B100 B17:B27</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Select Feature ID from Product Backlog" prompt="Exactly ONE team member may be responsible for any task, and they will receive grade credit for their work._x000a__x000a_If you have more than one person on your team, each member MUST select their initials for each task the agree to perform. Use this to ensure that " xr:uid="{00000000-0002-0000-0300-000002000000}">
+        <x14:dataValidation type="list" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Select Feature ID from Product Backlog" prompt="Exactly ONE team member may be responsible for any task, and they will receive grade credit for their work._x000a__x000a_If you have more than one person on your team, each member MUST select their initials for each task the agree to perform. Use this to ensure that " xr:uid="{00000000-0002-0000-0200-000002000000}">
           <x14:formula1>
             <xm:f>'Product Backlog'!$G$5:$G$8</xm:f>
           </x14:formula1>
           <x14:formula2>
             <xm:f>0</xm:f>
           </x14:formula2>
-          <xm:sqref>C17:C100</xm:sqref>
+          <xm:sqref>C29:C100 C17:C27</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -18992,13 +19181,13 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" customWidth="1"/>
-    <col min="3" max="3" width="12.28515625" customWidth="1"/>
-    <col min="4" max="4" width="51.85546875" customWidth="1"/>
-    <col min="5" max="5" width="17.7109375" customWidth="1"/>
-    <col min="6" max="6" width="51.85546875" customWidth="1"/>
+    <col min="1" max="1" width="10.33203125" customWidth="1"/>
+    <col min="3" max="3" width="12.33203125" customWidth="1"/>
+    <col min="4" max="4" width="51.83203125" customWidth="1"/>
+    <col min="5" max="5" width="17.6640625" customWidth="1"/>
+    <col min="6" max="6" width="51.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1024" s="29" customFormat="1" ht="18">
@@ -21095,13 +21284,13 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" customWidth="1"/>
-    <col min="3" max="3" width="12.28515625" customWidth="1"/>
-    <col min="4" max="4" width="51.85546875" customWidth="1"/>
-    <col min="5" max="5" width="17.7109375" customWidth="1"/>
-    <col min="6" max="6" width="51.85546875" customWidth="1"/>
+    <col min="1" max="1" width="10.33203125" customWidth="1"/>
+    <col min="3" max="3" width="12.33203125" customWidth="1"/>
+    <col min="4" max="4" width="51.83203125" customWidth="1"/>
+    <col min="5" max="5" width="17.6640625" customWidth="1"/>
+    <col min="6" max="6" width="51.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1024" s="29" customFormat="1" ht="18">
@@ -23199,13 +23388,13 @@
       <selection activeCell="G40" sqref="G40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" customWidth="1"/>
-    <col min="3" max="3" width="12.28515625" customWidth="1"/>
-    <col min="4" max="4" width="51.85546875" customWidth="1"/>
-    <col min="5" max="5" width="17.7109375" customWidth="1"/>
-    <col min="6" max="6" width="51.85546875" customWidth="1"/>
+    <col min="1" max="1" width="10.33203125" customWidth="1"/>
+    <col min="3" max="3" width="12.33203125" customWidth="1"/>
+    <col min="4" max="4" width="51.83203125" customWidth="1"/>
+    <col min="5" max="5" width="17.6640625" customWidth="1"/>
+    <col min="6" max="6" width="51.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1024" s="29" customFormat="1" ht="18">

</xml_diff>